<commit_message>
AFCM Screenshots added with code
</commit_message>
<xml_diff>
--- a/src/ANAD.xlsx
+++ b/src/ANAD.xlsx
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Type de véhicule, Référence, Spécifications, Fournisseur, Prix, Commentaires et évaluation (⭐) d'autres clients sur ces produits </t>
   </si>
   <si>
+    <t>En ligne</t>
+  </si>
+  <si>
     <t>Facebook, Ouedkniss</t>
   </si>
   <si>
@@ -44,9 +47,6 @@
   </si>
   <si>
     <t>Type de véhicule</t>
-  </si>
-  <si>
-    <t>En ligne</t>
   </si>
   <si>
     <t>Ouedkniss, Instagram</t>
@@ -86,12 +86,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Ruda"/>
     </font>
     <font>
       <color theme="1"/>
@@ -118,9 +123,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -343,9 +348,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="58.63"/>
-    <col customWidth="1" min="2" max="2" width="64.0"/>
-    <col customWidth="1" min="3" max="3" width="48.75"/>
+    <col customWidth="1" min="1" max="1" width="42.38"/>
+    <col customWidth="1" min="2" max="2" width="44.13"/>
+    <col customWidth="1" min="3" max="3" width="31.0"/>
     <col customWidth="1" min="4" max="4" width="95.75"/>
     <col customWidth="1" min="5" max="5" width="64.13"/>
     <col customWidth="1" min="6" max="6" width="48.25"/>
@@ -357,7 +362,7 @@
     <col customWidth="1" min="12" max="16" width="18.88"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="77.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -393,16 +398,16 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3">
         <v>4.0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -410,13 +415,13 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3">
         <v>2.0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -424,18 +429,18 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3">
         <v>3.0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>12</v>
@@ -452,7 +457,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
         <v>3.0</v>
@@ -463,10 +468,10 @@
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>3.0</v>
@@ -480,7 +485,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3">
         <v>2.0</v>
@@ -494,13 +499,13 @@
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3">
         <v>3.0</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +527,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" s="3">
         <v>3.0</v>
@@ -561,7 +566,7 @@
     </row>
     <row r="15">
       <c r="A15" s="3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>21</v>
@@ -570,7 +575,7 @@
         <v>2.0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16">
@@ -578,7 +583,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C16" s="3">
         <v>3.0</v>

</xml_diff>